<commit_message>
Added door direction tests to Adjacencies, created Adjacencies
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Desktop\eclipse-workspace\CluePaths\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C7A453-2FB3-4465-9E3E-3A0BD58E0FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C8F033-64F6-4227-8ABF-8680F744A3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="15" windowWidth="14220" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,8 +471,8 @@
   </sheetPr>
   <dimension ref="A1:AA1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finished the targets test
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Desktop\eclipse-workspace\CluePaths\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C8F033-64F6-4227-8ABF-8680F744A3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AF6DDF-1B7D-4F0A-A4B3-EACAB7442DA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="15" windowWidth="14220" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,10 +109,10 @@
     <t>Green: adjacency lists besides room entrance</t>
   </si>
   <si>
-    <t>Light Purple: walkway scenarios</t>
+    <t>Red: walkway scenarios</t>
   </si>
   <si>
-    <t>Light Blue: test targets</t>
+    <t>Pink: test targets</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +201,36 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF1155CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFC27BA0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFC27BA0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFC27BA0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -214,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,6 +279,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -471,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:AA1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -496,7 +541,7 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -769,13 +814,13 @@
       <c r="M4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="14" t="s">
         <v>3</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -1092,7 +1137,7 @@
       <c r="J8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1196,7 +1241,7 @@
       <c r="Q9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="17" t="s">
         <v>1</v>
       </c>
       <c r="S9" s="2" t="s">
@@ -1433,7 +1478,7 @@
       <c r="M12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="18" t="s">
         <v>1</v>
       </c>
       <c r="O12" s="2" t="s">
@@ -1489,7 +1534,7 @@
       <c r="D13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1608,7 +1653,7 @@
       <c r="P14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="17" t="s">
         <v>1</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -1990,7 +2035,7 @@
       <c r="E19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1999,7 +2044,7 @@
       <c r="H19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="18" t="s">
         <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -2112,7 +2157,7 @@
       <c r="R20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="S20" s="17" t="s">
         <v>1</v>
       </c>
       <c r="T20" s="2" t="s">
@@ -2177,7 +2222,7 @@
       <c r="L21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="16" t="s">
         <v>1</v>
       </c>
       <c r="N21" s="2" t="s">
@@ -2263,7 +2308,7 @@
       <c r="M22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="15" t="s">
         <v>18</v>
       </c>
       <c r="O22" s="3" t="s">
@@ -2488,7 +2533,7 @@
       <c r="E25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2521,7 +2566,7 @@
       <c r="P25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="3" t="s">
+      <c r="Q25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="R25" s="2" t="s">
@@ -2773,7 +2818,7 @@
       <c r="Q28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R28" s="2" t="s">
+      <c r="R28" s="17" t="s">
         <v>1</v>
       </c>
       <c r="S28" s="3" t="s">
@@ -4789,5 +4834,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got target tests working
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Desktop\eclipse-workspace\CluePaths\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AF6DDF-1B7D-4F0A-A4B3-EACAB7442DA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1325281B-DE9A-400A-BD57-03301257942A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="15" windowWidth="14220" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11535" yWindow="1200" windowWidth="14220" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +231,12 @@
         <bgColor rgb="FFC27BA0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF1155CC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,6 +300,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -516,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:AA1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -565,7 +574,7 @@
       <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -704,7 +713,7 @@
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1173,7 +1182,7 @@
       <c r="V8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W8" s="5" t="s">
+      <c r="W8" s="19" t="s">
         <v>7</v>
       </c>
       <c r="X8" s="5" t="s">
@@ -2044,7 +2053,7 @@
       <c r="H19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -2127,7 +2136,7 @@
       <c r="H20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="18" t="s">
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -2258,7 +2267,7 @@
       <c r="X21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y21" s="5" t="s">
+      <c r="Y21" s="19" t="s">
         <v>16</v>
       </c>
       <c r="Z21" s="3" t="s">

</xml_diff>